<commit_message>
renommer data ping et newdata
</commit_message>
<xml_diff>
--- a/data/pickle.xlsx
+++ b/data/pickle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phbro\Desktop\DOCUMENTS\ActuRank\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6446F92-CFCA-4948-9C0C-8CD4D286945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA57BB2F-535F-47F1-88B2-37E2B5846967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="62">
   <si>
     <t>players</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>28/08/2024</t>
+  </si>
+  <si>
+    <t>17/09/2024</t>
+  </si>
+  <si>
+    <t>25/09/2024</t>
   </si>
 </sst>
 </file>
@@ -609,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +737,7 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E35" si="0">IF(F4&gt;G4,1,0)</f>
+        <f t="shared" ref="E4:E48" si="0">IF(F4&gt;G4,1,0)</f>
         <v>1</v>
       </c>
       <c r="F4" s="5">
@@ -750,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="9" t="str">
-        <f t="shared" ref="K4:K35" si="1">IF(OR(OR(AND(OR(A4=B4,A4=C4,A4=D4,B4=C4,B4=D4,C4=D4),OR(A4&lt;&gt;"",D4&lt;&gt;"")),H4&gt;MAX(F4:G4),B4=C4),OR(AND(ISBLANK(A4)=FALSE,ISNA(VLOOKUP(A4,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B4,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C4,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D4)=FALSE,ISNA(VLOOKUP(D4,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A4:D4)=1,COUNTBLANK(A4:D4)=3))),"ERREUR","")</f>
+        <f t="shared" ref="K4:K48" si="1">IF(OR(OR(AND(OR(A4=B4,A4=C4,A4=D4,B4=C4,B4=D4,C4=D4),OR(A4&lt;&gt;"",D4&lt;&gt;"")),H4&gt;MAX(F4:G4),B4=C4),OR(AND(ISBLANK(A4)=FALSE,ISNA(VLOOKUP(A4,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B4,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C4,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D4)=FALSE,ISNA(VLOOKUP(D4,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A4:D4)=1,COUNTBLANK(A4:D4)=3))),"ERREUR","")</f>
         <v/>
       </c>
       <c r="L4" s="1"/>
@@ -1478,7 +1484,7 @@
         <v>59</v>
       </c>
       <c r="J21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K21" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1521,7 +1527,7 @@
         <v>59</v>
       </c>
       <c r="J22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1564,7 +1570,7 @@
         <v>59</v>
       </c>
       <c r="J23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K23" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1607,7 +1613,7 @@
         <v>59</v>
       </c>
       <c r="J24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1650,7 +1656,7 @@
         <v>59</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1687,7 +1693,7 @@
         <v>59</v>
       </c>
       <c r="J26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1724,7 +1730,7 @@
         <v>59</v>
       </c>
       <c r="J27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1761,7 +1767,7 @@
         <v>59</v>
       </c>
       <c r="J28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K28" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1798,7 +1804,7 @@
         <v>59</v>
       </c>
       <c r="J29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K29" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1835,7 +1841,7 @@
         <v>59</v>
       </c>
       <c r="J30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1872,7 +1878,7 @@
         <v>59</v>
       </c>
       <c r="J31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K31" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1909,7 +1915,7 @@
         <v>59</v>
       </c>
       <c r="J32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K32" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1946,7 +1952,7 @@
         <v>59</v>
       </c>
       <c r="J33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K33" s="9" t="str">
         <f t="shared" si="1"/>
@@ -1983,7 +1989,7 @@
         <v>59</v>
       </c>
       <c r="J34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K34" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2020,7 +2026,7 @@
         <v>59</v>
       </c>
       <c r="J35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K35" s="9" t="str">
         <f t="shared" si="1"/>
@@ -2033,16 +2039,36 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
+      <c r="B36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="9"/>
+      <c r="E36" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>11</v>
+      </c>
+      <c r="G36" s="5">
+        <v>9</v>
+      </c>
+      <c r="H36" s="1">
+        <v>11</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2</v>
+      </c>
+      <c r="K36" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2050,16 +2076,36 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
+      <c r="B37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="9"/>
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="5">
+        <v>12</v>
+      </c>
+      <c r="G37" s="5">
+        <v>10</v>
+      </c>
+      <c r="H37" s="1">
+        <v>11</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2</v>
+      </c>
+      <c r="K37" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -2067,16 +2113,36 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="9"/>
+      <c r="E38" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="5">
+        <v>11</v>
+      </c>
+      <c r="G38" s="5">
+        <v>7</v>
+      </c>
+      <c r="H38" s="1">
+        <v>11</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J38" s="1">
+        <v>2</v>
+      </c>
+      <c r="K38" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -2084,16 +2150,36 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
+      <c r="B39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="9"/>
+      <c r="E39" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>12</v>
+      </c>
+      <c r="G39" s="5">
+        <v>10</v>
+      </c>
+      <c r="H39" s="1">
+        <v>11</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J39" s="1">
+        <v>2</v>
+      </c>
+      <c r="K39" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -2101,16 +2187,36 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
+      <c r="B40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D40" s="7"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="9"/>
+      <c r="E40" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>12</v>
+      </c>
+      <c r="G40" s="5">
+        <v>10</v>
+      </c>
+      <c r="H40" s="1">
+        <v>11</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J40" s="1">
+        <v>2</v>
+      </c>
+      <c r="K40" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -2118,16 +2224,36 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
+      <c r="B41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="9"/>
+      <c r="E41" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>11</v>
+      </c>
+      <c r="G41" s="5">
+        <v>5</v>
+      </c>
+      <c r="H41" s="1">
+        <v>11</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J41" s="1">
+        <v>2</v>
+      </c>
+      <c r="K41" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -2135,16 +2261,36 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
+      <c r="B42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="9"/>
+      <c r="E42" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="5">
+        <v>11</v>
+      </c>
+      <c r="G42" s="5">
+        <v>9</v>
+      </c>
+      <c r="H42" s="1">
+        <v>11</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" s="1">
+        <v>2</v>
+      </c>
+      <c r="K42" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -2152,16 +2298,36 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
+      <c r="B43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D43" s="7"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="9"/>
+      <c r="E43" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F43" s="5">
+        <v>11</v>
+      </c>
+      <c r="G43" s="5">
+        <v>9</v>
+      </c>
+      <c r="H43" s="1">
+        <v>11</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2</v>
+      </c>
+      <c r="K43" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -2169,16 +2335,36 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
+      <c r="B44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D44" s="7"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="9"/>
+      <c r="E44" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="5">
+        <v>11</v>
+      </c>
+      <c r="G44" s="5">
+        <v>9</v>
+      </c>
+      <c r="H44" s="1">
+        <v>11</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J44" s="1">
+        <v>2</v>
+      </c>
+      <c r="K44" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -2186,16 +2372,36 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
+      <c r="B45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="9"/>
+      <c r="E45" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>13</v>
+      </c>
+      <c r="G45" s="5">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1">
+        <v>11</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J45" s="1">
+        <v>2</v>
+      </c>
+      <c r="K45" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -2203,16 +2409,36 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
+      <c r="B46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="9"/>
+      <c r="E46" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>12</v>
+      </c>
+      <c r="G46" s="5">
+        <v>10</v>
+      </c>
+      <c r="H46" s="1">
+        <v>11</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J46" s="1">
+        <v>2</v>
+      </c>
+      <c r="K46" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -2220,16 +2446,36 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
+      <c r="B47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D47" s="7"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="9"/>
+      <c r="E47" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F47" s="5">
+        <v>11</v>
+      </c>
+      <c r="G47" s="5">
+        <v>7</v>
+      </c>
+      <c r="H47" s="1">
+        <v>11</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J47" s="1">
+        <v>2</v>
+      </c>
+      <c r="K47" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
@@ -2237,16 +2483,36 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7"/>
+      <c r="B48" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="9"/>
+      <c r="E48" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F48" s="5">
+        <v>11</v>
+      </c>
+      <c r="G48" s="5">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1">
+        <v>11</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J48" s="1">
+        <v>2</v>
+      </c>
+      <c r="K48" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>

</xml_diff>

<commit_message>
newdata 6 nov 2024
</commit_message>
<xml_diff>
--- a/data/pickle.xlsx
+++ b/data/pickle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phbro\Desktop\DOCUMENTS\ActuRank\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF259459-8C18-413D-8FDF-EF4324DA8D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFE1A52-DF1F-4578-B370-44BC14EFE752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="70">
   <si>
     <t>players</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>22/10/2024</t>
+  </si>
+  <si>
+    <t>6/11/2024</t>
   </si>
 </sst>
 </file>
@@ -636,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95:I111"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3573,7 +3576,7 @@
         <v>21</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" ref="E75:E111" si="3">IF(F75&gt;G75,1,0)</f>
+        <f t="shared" ref="E75:E115" si="3">IF(F75&gt;G75,1,0)</f>
         <v>1</v>
       </c>
       <c r="F75" s="5">
@@ -4327,7 +4330,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="9" t="str">
-        <f t="shared" ref="K94:K111" si="5">IF(OR(OR(AND(OR(A94=B94,A94=C94,A94=D94,B94=C94,B94=D94,C94=D94),OR(A94&lt;&gt;"",D94&lt;&gt;"")),H94&gt;MAX(F94:G94),B94=C94),OR(AND(ISBLANK(A94)=FALSE,ISNA(VLOOKUP(A94,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B94,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C94,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D94)=FALSE,ISNA(VLOOKUP(D94,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A94:D94)=1,COUNTBLANK(A94:D94)=3))),"ERREUR","")</f>
+        <f t="shared" ref="K94:K115" si="5">IF(OR(OR(AND(OR(A94=B94,A94=C94,A94=D94,B94=C94,B94=D94,C94=D94),OR(A94&lt;&gt;"",D94&lt;&gt;"")),H94&gt;MAX(F94:G94),B94=C94),OR(AND(ISBLANK(A94)=FALSE,ISNA(VLOOKUP(A94,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B94,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C94,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D94)=FALSE,ISNA(VLOOKUP(D94,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A94:D94)=1,COUNTBLANK(A94:D94)=3))),"ERREUR","")</f>
         <v/>
       </c>
       <c r="L94" s="1"/>
@@ -4966,16 +4969,36 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
-      <c r="B112" s="6"/>
-      <c r="C112" s="7"/>
+      <c r="B112" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D112" s="7"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="K112" s="9"/>
+      <c r="E112" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F112" s="5">
+        <v>12</v>
+      </c>
+      <c r="G112" s="5">
+        <v>10</v>
+      </c>
+      <c r="H112" s="1">
+        <v>11</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J112" s="1">
+        <v>2</v>
+      </c>
+      <c r="K112" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
@@ -4983,16 +5006,36 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
-      <c r="B113" s="6"/>
-      <c r="C113" s="7"/>
+      <c r="B113" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D113" s="7"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="1"/>
-      <c r="J113" s="1"/>
-      <c r="K113" s="9"/>
+      <c r="E113" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F113" s="5">
+        <v>11</v>
+      </c>
+      <c r="G113" s="5">
+        <v>8</v>
+      </c>
+      <c r="H113" s="1">
+        <v>11</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J113" s="1">
+        <v>2</v>
+      </c>
+      <c r="K113" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
@@ -5000,16 +5043,36 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
-      <c r="B114" s="6"/>
-      <c r="C114" s="7"/>
+      <c r="B114" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D114" s="7"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="1"/>
-      <c r="J114" s="1"/>
-      <c r="K114" s="9"/>
+      <c r="E114" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F114" s="5">
+        <v>11</v>
+      </c>
+      <c r="G114" s="5">
+        <v>7</v>
+      </c>
+      <c r="H114" s="1">
+        <v>11</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J114" s="1">
+        <v>2</v>
+      </c>
+      <c r="K114" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
@@ -5017,16 +5080,36 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
-      <c r="B115" s="6"/>
-      <c r="C115" s="7"/>
+      <c r="B115" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D115" s="7"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1"/>
-      <c r="J115" s="1"/>
-      <c r="K115" s="9"/>
+      <c r="E115" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F115" s="5">
+        <v>11</v>
+      </c>
+      <c r="G115" s="5">
+        <v>6</v>
+      </c>
+      <c r="H115" s="1">
+        <v>11</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J115" s="1">
+        <v>2</v>
+      </c>
+      <c r="K115" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>

</xml_diff>